<commit_message>
massdelete section upd, current groups displayed
</commit_message>
<xml_diff>
--- a/testMassDelete.xlsx
+++ b/testMassDelete.xlsx
@@ -4,26 +4,45 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="MassDelete" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>maurizio.accordino@hpe.com</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+  <si>
+    <t>vstoyanov@hpe.com</t>
+  </si>
+  <si>
+    <t>simeons@hpe.com</t>
+  </si>
+  <si>
+    <t>bogomolov@hpe.com</t>
+  </si>
+  <si>
+    <t>Cannot get user groups</t>
+  </si>
+  <si>
+    <t>asdasdsa</t>
+  </si>
+  <si>
+    <t>simeons@hpe.com delete</t>
+  </si>
+  <si>
+    <t>asdasdsa delete</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -38,6 +57,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -63,8 +88,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -370,92 +397,112 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A23"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="57" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>